<commit_message>
add future category ranking interface
</commit_message>
<xml_diff>
--- a/data/future.xlsx
+++ b/data/future.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\belinda\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\smda\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,45 +23,12 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>洗发沐浴</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>卫生巾/护垫/成人尿裤</t>
-  </si>
-  <si>
-    <t>家私/皮具护理品</t>
-  </si>
-  <si>
-    <t>香熏用品</t>
-  </si>
-  <si>
-    <t>纸品/湿巾</t>
-  </si>
-  <si>
-    <t>家庭环境清洁剂</t>
-  </si>
-  <si>
-    <t>驱虫用品</t>
-  </si>
-  <si>
-    <t>衣物清洁剂/护理剂</t>
-  </si>
-  <si>
-    <t>室内除臭/芳香用品</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,28 +49,6 @@
       <color theme="1"/>
       <name val="等线"/>
       <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="微软雅黑"/>
-      <family val="2"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="微软雅黑"/>
-      <family val="2"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -133,17 +78,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -427,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection sqref="A1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -438,109 +377,67 @@
     <col min="1" max="9" width="13.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="1">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="1">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="1">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="1">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3"/>
     </row>
-    <row r="2" spans="1:10" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
-        <v>85785156</v>
-      </c>
-      <c r="B2" s="2">
-        <v>13496245</v>
-      </c>
-      <c r="C2" s="2">
-        <v>9857561</v>
-      </c>
-      <c r="D2" s="2">
-        <v>6695425</v>
-      </c>
-      <c r="E2" s="2">
-        <v>7177597</v>
-      </c>
-      <c r="F2" s="2">
-        <v>7289906</v>
-      </c>
-      <c r="G2" s="2">
-        <v>4851625</v>
-      </c>
-      <c r="H2" s="2">
-        <v>6148268</v>
-      </c>
-      <c r="I2" s="2">
-        <v>3746208</v>
-      </c>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>635333980</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B2" s="1">
+        <v>297083785</v>
+      </c>
+      <c r="C2" s="1">
         <v>141679615</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D2" s="1">
+        <v>130143905</v>
+      </c>
+      <c r="E2" s="1">
+        <v>115280370</v>
+      </c>
+      <c r="F2" s="1">
+        <v>79968760</v>
+      </c>
+      <c r="G2" s="1">
         <v>70457945</v>
       </c>
-      <c r="D3" s="2">
+      <c r="H2" s="1">
         <v>56205570</v>
       </c>
-      <c r="E3" s="2">
-        <v>297083785</v>
-      </c>
-      <c r="F3" s="2">
-        <v>115280370</v>
-      </c>
-      <c r="G3" s="2">
+      <c r="I2" s="1">
         <v>27251910</v>
       </c>
-      <c r="H3" s="2">
-        <v>130143905</v>
-      </c>
-      <c r="I3" s="2">
-        <v>79968760</v>
-      </c>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>